<commit_message>
Cập nhật thông tin người và ngày thực hiện sửa lỗi
</commit_message>
<xml_diff>
--- a/BaoCao_Review/FD/[Team1][RV_FD]QLNhaPP_QLTaiKhoan_QLDoiTraHangHoa.xlsx
+++ b/BaoCao_Review/FD/[Team1][RV_FD]QLNhaPP_QLTaiKhoan_QLDoiTraHangHoa.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18201"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Học tập\Học kỳ 7\PT Ứng dụng HTTT hiện đại\Đồ án\TH2014-1-PTUDHTTTHD-SaveMyLife-SML\BaoCao_Review\FD\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Semester 7\PTUD HTTT\Project\TH2014-1-PTUDHTTTHD-SaveMyLife-SML\BaoCao_Review\FD\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -25,12 +25,12 @@
     <definedName name="_xlnm.Print_Area" localSheetId="4">'Template Revision history'!$A$1:$F$26</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="1">'Walk-through'!$A$1:$Y$127</definedName>
   </definedNames>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="171027"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1080" uniqueCount="343">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1081" uniqueCount="343">
   <si>
     <t>Inform to:</t>
   </si>
@@ -1477,9 +1477,6 @@
     <t>Giai đoạn:</t>
   </si>
   <si>
-    <t>Phân tích</t>
-  </si>
-  <si>
     <t>Mã số tài liệu</t>
   </si>
   <si>
@@ -1724,12 +1721,15 @@
   </si>
   <si>
     <t>Sửa kiểu dữ liệu trong hàm getCongNo của class NhaPhanPhoi</t>
+  </si>
+  <si>
+    <t>Thiết kế</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="10">
     <numFmt numFmtId="164" formatCode="0_);[Red]\(0\)"/>
     <numFmt numFmtId="165" formatCode="0.00_ "/>
@@ -3358,14 +3358,14 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" shrinkToFit="1"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center" wrapText="1" shrinkToFit="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" shrinkToFit="1"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
       <protection locked="0"/>
@@ -3373,15 +3373,6 @@
     <xf numFmtId="0" fontId="23" fillId="3" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
       <protection locked="0"/>
@@ -3397,6 +3388,15 @@
     <xf numFmtId="0" fontId="23" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
     </xf>
+    <xf numFmtId="0" fontId="23" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -3441,18 +3441,6 @@
     </xf>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="23" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="171" fontId="23" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
@@ -3596,6 +3584,18 @@
     <xf numFmtId="172" fontId="23" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="23" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="23" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="23" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -4394,7 +4394,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="11">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Bình thường" xfId="0" builtinId="0"/>
     <cellStyle name="標準 2" xfId="1"/>
     <cellStyle name="標準 3" xfId="9"/>
     <cellStyle name="標準 4" xfId="10"/>
@@ -5056,7 +5056,7 @@
         <xdr:cNvPr id="6145" name="正方形/長方形 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000001180000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000001180000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5124,7 +5124,7 @@
         <xdr:cNvPr id="6146" name="正方形/長方形 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000002180000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000002180000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -6331,7 +6331,7 @@
         <xdr:cNvPr id="6147" name="正方形/長方形 12">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000003180000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000003180000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -6506,7 +6506,7 @@
         <xdr:cNvPr id="10" name="正方形/長方形 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-00000A000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-00000A000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -8155,7 +8155,7 @@
         <xdr:cNvPr id="11" name="正方形/長方形 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-00000B000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-00000B000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -11532,7 +11532,7 @@
         <xdr:cNvPr id="15" name="正方形/長方形 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{EF028B0C-D360-49E4-8A51-5DDD9991BE88}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EF028B0C-D360-49E4-8A51-5DDD9991BE88}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -11934,7 +11934,7 @@
         <xdr:cNvPr id="7169" name="正方形/長方形 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-0000011C0000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-0000011C0000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -12002,7 +12002,7 @@
         <xdr:cNvPr id="7170" name="正方形/長方形 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-0000021C0000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-0000021C0000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -12965,7 +12965,7 @@
         <xdr:cNvPr id="10" name="正方形/長方形 12">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-00000A000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-00000A000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -13140,7 +13140,7 @@
         <xdr:cNvPr id="11" name="正方形/長方形 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-00000B000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-00000B000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -14796,7 +14796,7 @@
         <xdr:cNvPr id="8" name="正方形/長方形 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000008000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000008000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -16930,7 +16930,7 @@
         <xdr:cNvPr id="9" name="正方形/長方形 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{1D8941C5-C0B8-4AFE-9187-051FAF622739}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1D8941C5-C0B8-4AFE-9187-051FAF622739}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -17332,7 +17332,7 @@
         <xdr:cNvPr id="2" name="正方形/長方形 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{79A14699-8D8D-4528-A314-7338B8F61820}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{79A14699-8D8D-4528-A314-7338B8F61820}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -17396,22 +17396,6 @@
             </a:rPr>
             <a:t>■Additional description</a:t>
           </a:r>
-          <a:r>
-            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="900" b="0" i="0" u="none" strike="noStrike" kern="0" cap="none" spc="0" normalizeH="0" baseline="0" noProof="0">
-              <a:ln>
-                <a:noFill/>
-              </a:ln>
-              <a:solidFill>
-                <a:schemeClr val="accent1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:uLnTx/>
-              <a:uFillTx/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-            </a:rPr>
-            <a:t/>
-          </a:r>
           <a:br>
             <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="900" b="0" i="0" u="none" strike="noStrike" kern="0" cap="none" spc="0" normalizeH="0" baseline="0" noProof="0">
               <a:ln>
@@ -18183,7 +18167,7 @@
         <xdr:cNvPr id="3" name="正方形/長方形 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{1A8EF14B-5FF3-47E1-8D9B-66E826AF88DF}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1A8EF14B-5FF3-47E1-8D9B-66E826AF88DF}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -18381,15 +18365,6 @@
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
             <a:t>", or "N/A.</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="900" b="0" i="0" baseline="0">
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="ＭＳ Ｐゴシック" panose="020B0600070205080204" pitchFamily="50" charset="-128"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t/>
           </a:r>
           <a:br>
             <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="900" b="0" i="0" baseline="0">
@@ -18768,6 +18743,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -18803,6 +18795,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -18985,8 +18994,8 @@
   </sheetPr>
   <dimension ref="A1:AN82"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" view="pageBreakPreview" topLeftCell="A27" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="D39" sqref="D39"/>
+    <sheetView showGridLines="0" tabSelected="1" view="pageBreakPreview" topLeftCell="A34" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="B32" sqref="B32:B39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -19014,10 +19023,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="15" customHeight="1">
-      <c r="B1" s="340"/>
-      <c r="C1" s="341"/>
-      <c r="D1" s="341"/>
-      <c r="E1" s="341"/>
+      <c r="B1" s="336"/>
+      <c r="C1" s="337"/>
+      <c r="D1" s="337"/>
+      <c r="E1" s="337"/>
       <c r="F1" s="210"/>
       <c r="G1" s="211"/>
       <c r="H1" s="211"/>
@@ -19030,12 +19039,12 @@
       <c r="O1" s="211"/>
       <c r="P1" s="212"/>
       <c r="Q1" s="285" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="R1" s="286"/>
       <c r="S1" s="287"/>
       <c r="T1" s="285" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="U1" s="286"/>
       <c r="V1" s="286"/>
@@ -19045,10 +19054,10 @@
       <c r="Z1" s="213"/>
     </row>
     <row r="2" spans="1:26" ht="15" customHeight="1">
-      <c r="B2" s="323"/>
+      <c r="B2" s="319"/>
       <c r="C2" s="298"/>
       <c r="D2" s="298"/>
-      <c r="E2" s="324"/>
+      <c r="E2" s="320"/>
       <c r="F2" s="215"/>
       <c r="G2" s="216"/>
       <c r="H2" s="216"/>
@@ -19061,25 +19070,25 @@
       <c r="O2" s="216"/>
       <c r="P2" s="217"/>
       <c r="Q2" s="285" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="R2" s="286"/>
       <c r="S2" s="287"/>
-      <c r="T2" s="320" t="s">
-        <v>294</v>
-      </c>
-      <c r="U2" s="321"/>
-      <c r="V2" s="321"/>
-      <c r="W2" s="321"/>
-      <c r="X2" s="321"/>
-      <c r="Y2" s="322"/>
+      <c r="T2" s="316" t="s">
+        <v>293</v>
+      </c>
+      <c r="U2" s="317"/>
+      <c r="V2" s="317"/>
+      <c r="W2" s="317"/>
+      <c r="X2" s="317"/>
+      <c r="Y2" s="318"/>
       <c r="Z2" s="213"/>
     </row>
     <row r="3" spans="1:26" ht="15" customHeight="1">
-      <c r="B3" s="323"/>
+      <c r="B3" s="319"/>
       <c r="C3" s="298"/>
       <c r="D3" s="298"/>
-      <c r="E3" s="324"/>
+      <c r="E3" s="320"/>
       <c r="F3" s="215"/>
       <c r="G3" s="288" t="s">
         <v>257</v>
@@ -19087,7 +19096,7 @@
       <c r="H3" s="288"/>
       <c r="I3" s="288"/>
       <c r="J3" s="288" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="K3" s="288"/>
       <c r="L3" s="288"/>
@@ -19096,25 +19105,25 @@
       <c r="O3" s="288"/>
       <c r="P3" s="217"/>
       <c r="Q3" s="285" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="R3" s="286"/>
       <c r="S3" s="287"/>
-      <c r="T3" s="342" t="s">
-        <v>291</v>
-      </c>
-      <c r="U3" s="343"/>
-      <c r="V3" s="343"/>
-      <c r="W3" s="343"/>
-      <c r="X3" s="343"/>
-      <c r="Y3" s="344"/>
+      <c r="T3" s="338" t="s">
+        <v>290</v>
+      </c>
+      <c r="U3" s="339"/>
+      <c r="V3" s="339"/>
+      <c r="W3" s="339"/>
+      <c r="X3" s="339"/>
+      <c r="Y3" s="340"/>
       <c r="Z3" s="213"/>
     </row>
     <row r="4" spans="1:26" ht="15" customHeight="1">
-      <c r="B4" s="323"/>
+      <c r="B4" s="319"/>
       <c r="C4" s="298"/>
       <c r="D4" s="298"/>
-      <c r="E4" s="324"/>
+      <c r="E4" s="320"/>
       <c r="F4" s="218"/>
       <c r="G4" s="219"/>
       <c r="H4" s="220"/>
@@ -19127,25 +19136,25 @@
       <c r="O4" s="220"/>
       <c r="P4" s="221"/>
       <c r="Q4" s="289" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="R4" s="290"/>
       <c r="S4" s="291"/>
-      <c r="T4" s="327" t="s">
-        <v>292</v>
-      </c>
-      <c r="U4" s="328"/>
-      <c r="V4" s="328"/>
-      <c r="W4" s="328"/>
-      <c r="X4" s="328"/>
-      <c r="Y4" s="329"/>
+      <c r="T4" s="323" t="s">
+        <v>291</v>
+      </c>
+      <c r="U4" s="324"/>
+      <c r="V4" s="324"/>
+      <c r="W4" s="324"/>
+      <c r="X4" s="324"/>
+      <c r="Y4" s="325"/>
       <c r="Z4" s="213"/>
     </row>
     <row r="5" spans="1:26" ht="15" customHeight="1">
-      <c r="B5" s="323"/>
+      <c r="B5" s="319"/>
       <c r="C5" s="298"/>
       <c r="D5" s="298"/>
-      <c r="E5" s="324"/>
+      <c r="E5" s="320"/>
       <c r="F5" s="222"/>
       <c r="G5" s="288" t="s">
         <v>258</v>
@@ -19153,7 +19162,7 @@
       <c r="H5" s="288"/>
       <c r="I5" s="288"/>
       <c r="J5" s="298" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="K5" s="298"/>
       <c r="L5" s="298"/>
@@ -19164,19 +19173,19 @@
       <c r="Q5" s="292"/>
       <c r="R5" s="293"/>
       <c r="S5" s="294"/>
-      <c r="T5" s="330"/>
-      <c r="U5" s="331"/>
-      <c r="V5" s="331"/>
-      <c r="W5" s="331"/>
-      <c r="X5" s="331"/>
-      <c r="Y5" s="332"/>
+      <c r="T5" s="326"/>
+      <c r="U5" s="327"/>
+      <c r="V5" s="327"/>
+      <c r="W5" s="327"/>
+      <c r="X5" s="327"/>
+      <c r="Y5" s="328"/>
       <c r="Z5" s="213"/>
     </row>
     <row r="6" spans="1:26" ht="15" customHeight="1">
-      <c r="B6" s="323"/>
+      <c r="B6" s="319"/>
       <c r="C6" s="298"/>
       <c r="D6" s="298"/>
-      <c r="E6" s="324"/>
+      <c r="E6" s="320"/>
       <c r="F6" s="224"/>
       <c r="G6" s="225"/>
       <c r="H6" s="225"/>
@@ -19191,19 +19200,19 @@
       <c r="Q6" s="295"/>
       <c r="R6" s="296"/>
       <c r="S6" s="297"/>
-      <c r="T6" s="333"/>
-      <c r="U6" s="334"/>
-      <c r="V6" s="334"/>
-      <c r="W6" s="334"/>
-      <c r="X6" s="334"/>
-      <c r="Y6" s="335"/>
+      <c r="T6" s="329"/>
+      <c r="U6" s="330"/>
+      <c r="V6" s="330"/>
+      <c r="W6" s="330"/>
+      <c r="X6" s="330"/>
+      <c r="Y6" s="331"/>
       <c r="Z6" s="213"/>
     </row>
     <row r="7" spans="1:26" ht="15" customHeight="1">
-      <c r="B7" s="323"/>
+      <c r="B7" s="319"/>
       <c r="C7" s="298"/>
       <c r="D7" s="298"/>
-      <c r="E7" s="324"/>
+      <c r="E7" s="320"/>
       <c r="F7" s="215"/>
       <c r="G7" s="216"/>
       <c r="H7" s="220"/>
@@ -19219,22 +19228,22 @@
       <c r="R7" s="211"/>
       <c r="S7" s="212"/>
       <c r="T7" s="285" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="U7" s="286"/>
       <c r="V7" s="287"/>
       <c r="W7" s="285" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="X7" s="286"/>
       <c r="Y7" s="287"/>
       <c r="Z7" s="213"/>
     </row>
     <row r="8" spans="1:26" ht="15" customHeight="1">
-      <c r="B8" s="323"/>
+      <c r="B8" s="319"/>
       <c r="C8" s="298"/>
       <c r="D8" s="298"/>
-      <c r="E8" s="324"/>
+      <c r="E8" s="320"/>
       <c r="F8" s="215"/>
       <c r="G8" s="288"/>
       <c r="H8" s="288"/>
@@ -19249,21 +19258,23 @@
       <c r="Q8" s="216"/>
       <c r="R8" s="216"/>
       <c r="S8" s="217"/>
-      <c r="T8" s="289"/>
+      <c r="T8" s="289" t="s">
+        <v>301</v>
+      </c>
       <c r="U8" s="290"/>
       <c r="V8" s="291"/>
       <c r="W8" s="289" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="X8" s="290"/>
       <c r="Y8" s="291"/>
       <c r="Z8" s="213"/>
     </row>
     <row r="9" spans="1:26" ht="15" customHeight="1">
-      <c r="B9" s="323"/>
+      <c r="B9" s="319"/>
       <c r="C9" s="298"/>
       <c r="D9" s="298"/>
-      <c r="E9" s="324"/>
+      <c r="E9" s="320"/>
       <c r="F9" s="215"/>
       <c r="J9" s="216"/>
       <c r="K9" s="216"/>
@@ -19284,10 +19295,10 @@
       <c r="Z9" s="213"/>
     </row>
     <row r="10" spans="1:26" ht="15" customHeight="1">
-      <c r="B10" s="323"/>
+      <c r="B10" s="319"/>
       <c r="C10" s="298"/>
       <c r="D10" s="298"/>
-      <c r="E10" s="324"/>
+      <c r="E10" s="320"/>
       <c r="F10" s="215"/>
       <c r="G10" s="288" t="s">
         <v>259</v>
@@ -19295,7 +19306,7 @@
       <c r="H10" s="288"/>
       <c r="I10" s="288"/>
       <c r="J10" s="288" t="s">
-        <v>260</v>
+        <v>342</v>
       </c>
       <c r="K10" s="288"/>
       <c r="L10" s="288"/>
@@ -19315,10 +19326,10 @@
       <c r="Z10" s="213"/>
     </row>
     <row r="11" spans="1:26" ht="15" customHeight="1">
-      <c r="B11" s="323"/>
+      <c r="B11" s="319"/>
       <c r="C11" s="298"/>
       <c r="D11" s="298"/>
-      <c r="E11" s="324"/>
+      <c r="E11" s="320"/>
       <c r="F11" s="215"/>
       <c r="G11" s="216"/>
       <c r="H11" s="216"/>
@@ -19342,10 +19353,10 @@
       <c r="Z11" s="213"/>
     </row>
     <row r="12" spans="1:26" ht="15" customHeight="1">
-      <c r="B12" s="325"/>
+      <c r="B12" s="321"/>
       <c r="C12" s="299"/>
       <c r="D12" s="299"/>
-      <c r="E12" s="326"/>
+      <c r="E12" s="322"/>
       <c r="F12" s="228"/>
       <c r="G12" s="229"/>
       <c r="H12" s="229"/>
@@ -19410,107 +19421,107 @@
       <c r="Z14" s="231"/>
     </row>
     <row r="15" spans="1:26" s="209" customFormat="1" ht="27" customHeight="1">
-      <c r="B15" s="336" t="s">
-        <v>267</v>
-      </c>
-      <c r="C15" s="337"/>
-      <c r="D15" s="337"/>
-      <c r="E15" s="338"/>
-      <c r="F15" s="339"/>
-      <c r="G15" s="339"/>
-      <c r="H15" s="339"/>
-      <c r="I15" s="339"/>
-      <c r="J15" s="339"/>
-      <c r="K15" s="339"/>
-      <c r="L15" s="339"/>
-      <c r="M15" s="339"/>
-      <c r="N15" s="339"/>
-      <c r="O15" s="339"/>
-      <c r="P15" s="339"/>
-      <c r="Q15" s="339"/>
-      <c r="R15" s="339"/>
-      <c r="S15" s="339"/>
-      <c r="T15" s="339"/>
-      <c r="U15" s="339"/>
-      <c r="V15" s="339"/>
-      <c r="W15" s="339"/>
-      <c r="X15" s="339"/>
-      <c r="Y15" s="339"/>
+      <c r="B15" s="332" t="s">
+        <v>266</v>
+      </c>
+      <c r="C15" s="333"/>
+      <c r="D15" s="333"/>
+      <c r="E15" s="334"/>
+      <c r="F15" s="335"/>
+      <c r="G15" s="335"/>
+      <c r="H15" s="335"/>
+      <c r="I15" s="335"/>
+      <c r="J15" s="335"/>
+      <c r="K15" s="335"/>
+      <c r="L15" s="335"/>
+      <c r="M15" s="335"/>
+      <c r="N15" s="335"/>
+      <c r="O15" s="335"/>
+      <c r="P15" s="335"/>
+      <c r="Q15" s="335"/>
+      <c r="R15" s="335"/>
+      <c r="S15" s="335"/>
+      <c r="T15" s="335"/>
+      <c r="U15" s="335"/>
+      <c r="V15" s="335"/>
+      <c r="W15" s="335"/>
+      <c r="X15" s="335"/>
+      <c r="Y15" s="335"/>
       <c r="Z15" s="233"/>
     </row>
     <row r="16" spans="1:26" s="235" customFormat="1" ht="39.75" customHeight="1">
       <c r="A16" s="234"/>
-      <c r="B16" s="305" t="s">
+      <c r="B16" s="301" t="s">
+        <v>267</v>
+      </c>
+      <c r="C16" s="302"/>
+      <c r="D16" s="302"/>
+      <c r="E16" s="303"/>
+      <c r="F16" s="280" t="s">
         <v>268</v>
       </c>
-      <c r="C16" s="306"/>
-      <c r="D16" s="306"/>
-      <c r="E16" s="307"/>
-      <c r="F16" s="283" t="s">
+      <c r="G16" s="280"/>
+      <c r="H16" s="279" t="s">
+        <v>298</v>
+      </c>
+      <c r="I16" s="279"/>
+      <c r="J16" s="280" t="s">
         <v>269</v>
       </c>
-      <c r="G16" s="283"/>
-      <c r="H16" s="282" t="s">
-        <v>299</v>
-      </c>
-      <c r="I16" s="282"/>
-      <c r="J16" s="283" t="s">
+      <c r="K16" s="280"/>
+      <c r="L16" s="279" t="s">
+        <v>297</v>
+      </c>
+      <c r="M16" s="279"/>
+      <c r="N16" s="280" t="s">
         <v>270</v>
       </c>
-      <c r="K16" s="283"/>
-      <c r="L16" s="282" t="s">
-        <v>298</v>
-      </c>
-      <c r="M16" s="282"/>
-      <c r="N16" s="283" t="s">
+      <c r="O16" s="280"/>
+      <c r="P16" s="278"/>
+      <c r="Q16" s="278"/>
+      <c r="R16" s="281" t="s">
         <v>271</v>
       </c>
-      <c r="O16" s="283"/>
-      <c r="P16" s="281"/>
-      <c r="Q16" s="281"/>
-      <c r="R16" s="284" t="s">
+      <c r="S16" s="281"/>
+      <c r="T16" s="281"/>
+      <c r="U16" s="345" t="s">
         <v>272</v>
       </c>
-      <c r="S16" s="284"/>
-      <c r="T16" s="284"/>
-      <c r="U16" s="300" t="s">
-        <v>273</v>
-      </c>
-      <c r="V16" s="301"/>
-      <c r="W16" s="301"/>
-      <c r="X16" s="301"/>
-      <c r="Y16" s="302"/>
+      <c r="V16" s="346"/>
+      <c r="W16" s="346"/>
+      <c r="X16" s="346"/>
+      <c r="Y16" s="347"/>
     </row>
     <row r="17" spans="1:40" s="235" customFormat="1" ht="39" customHeight="1">
       <c r="A17" s="234"/>
-      <c r="B17" s="308"/>
-      <c r="C17" s="309"/>
-      <c r="D17" s="309"/>
-      <c r="E17" s="310"/>
-      <c r="F17" s="283" t="s">
-        <v>274</v>
-      </c>
-      <c r="G17" s="283"/>
-      <c r="H17" s="345" t="s">
-        <v>297</v>
-      </c>
-      <c r="I17" s="346"/>
-      <c r="J17" s="346"/>
-      <c r="K17" s="346"/>
-      <c r="L17" s="346"/>
-      <c r="M17" s="346"/>
-      <c r="N17" s="346"/>
-      <c r="O17" s="346"/>
-      <c r="P17" s="346"/>
-      <c r="Q17" s="347"/>
-      <c r="R17" s="275"/>
-      <c r="S17" s="275"/>
-      <c r="T17" s="275"/>
-      <c r="U17" s="274">
+      <c r="B17" s="304"/>
+      <c r="C17" s="305"/>
+      <c r="D17" s="305"/>
+      <c r="E17" s="306"/>
+      <c r="F17" s="280" t="s">
+        <v>273</v>
+      </c>
+      <c r="G17" s="280"/>
+      <c r="H17" s="341" t="s">
+        <v>296</v>
+      </c>
+      <c r="I17" s="342"/>
+      <c r="J17" s="342"/>
+      <c r="K17" s="342"/>
+      <c r="L17" s="342"/>
+      <c r="M17" s="342"/>
+      <c r="N17" s="342"/>
+      <c r="O17" s="342"/>
+      <c r="P17" s="342"/>
+      <c r="Q17" s="343"/>
+      <c r="R17" s="274"/>
+      <c r="S17" s="274"/>
+      <c r="T17" s="274"/>
+      <c r="U17" s="275">
         <v>12</v>
       </c>
-      <c r="V17" s="274"/>
-      <c r="W17" s="274"/>
+      <c r="V17" s="275"/>
+      <c r="W17" s="275"/>
       <c r="X17" s="273" t="s">
         <v>254</v>
       </c>
@@ -19518,42 +19529,42 @@
     </row>
     <row r="18" spans="1:40" s="235" customFormat="1" ht="40.700000000000003" customHeight="1">
       <c r="A18" s="234"/>
-      <c r="B18" s="312" t="s">
+      <c r="B18" s="308" t="s">
         <v>17</v>
       </c>
-      <c r="C18" s="313"/>
-      <c r="D18" s="313"/>
-      <c r="E18" s="314"/>
-      <c r="F18" s="303" t="s">
+      <c r="C18" s="309"/>
+      <c r="D18" s="309"/>
+      <c r="E18" s="310"/>
+      <c r="F18" s="348" t="s">
+        <v>274</v>
+      </c>
+      <c r="G18" s="348"/>
+      <c r="H18" s="312" t="s">
+        <v>308</v>
+      </c>
+      <c r="I18" s="312"/>
+      <c r="J18" s="307" t="s">
         <v>275</v>
       </c>
-      <c r="G18" s="303"/>
-      <c r="H18" s="316" t="s">
-        <v>309</v>
-      </c>
-      <c r="I18" s="316"/>
-      <c r="J18" s="311" t="s">
+      <c r="K18" s="307"/>
+      <c r="L18" s="312" t="s">
+        <v>308</v>
+      </c>
+      <c r="M18" s="312"/>
+      <c r="N18" s="282" t="s">
         <v>276</v>
       </c>
-      <c r="K18" s="311"/>
-      <c r="L18" s="316" t="s">
-        <v>309</v>
-      </c>
-      <c r="M18" s="316"/>
-      <c r="N18" s="278" t="s">
-        <v>277</v>
-      </c>
-      <c r="O18" s="278"/>
-      <c r="P18" s="348">
+      <c r="O18" s="282"/>
+      <c r="P18" s="344">
         <v>3</v>
       </c>
-      <c r="Q18" s="348"/>
-      <c r="R18" s="275"/>
-      <c r="S18" s="275"/>
-      <c r="T18" s="275"/>
-      <c r="U18" s="274"/>
-      <c r="V18" s="274"/>
-      <c r="W18" s="274"/>
+      <c r="Q18" s="344"/>
+      <c r="R18" s="274"/>
+      <c r="S18" s="274"/>
+      <c r="T18" s="274"/>
+      <c r="U18" s="275"/>
+      <c r="V18" s="275"/>
+      <c r="W18" s="275"/>
       <c r="X18" s="273"/>
       <c r="Y18" s="273"/>
     </row>
@@ -19565,47 +19576,47 @@
       <c r="C19" s="277"/>
       <c r="D19" s="277"/>
       <c r="E19" s="277"/>
-      <c r="F19" s="278" t="s">
+      <c r="F19" s="282" t="s">
+        <v>277</v>
+      </c>
+      <c r="G19" s="282"/>
+      <c r="H19" s="300" t="s">
+        <v>293</v>
+      </c>
+      <c r="I19" s="300"/>
+      <c r="J19" s="315" t="s">
         <v>278</v>
       </c>
-      <c r="G19" s="278"/>
-      <c r="H19" s="304" t="s">
-        <v>294</v>
-      </c>
-      <c r="I19" s="304"/>
-      <c r="J19" s="319" t="s">
+      <c r="K19" s="315"/>
+      <c r="L19" s="311">
+        <v>0.875</v>
+      </c>
+      <c r="M19" s="311"/>
+      <c r="N19" s="282" t="s">
         <v>279</v>
       </c>
-      <c r="K19" s="319"/>
-      <c r="L19" s="315">
-        <v>0.875</v>
-      </c>
-      <c r="M19" s="315"/>
-      <c r="N19" s="278" t="s">
-        <v>280</v>
-      </c>
-      <c r="O19" s="278"/>
-      <c r="P19" s="317">
+      <c r="O19" s="282"/>
+      <c r="P19" s="313">
         <v>0.95833333333333337</v>
       </c>
-      <c r="Q19" s="318"/>
-      <c r="R19" s="275"/>
-      <c r="S19" s="275"/>
-      <c r="T19" s="275"/>
-      <c r="U19" s="274"/>
-      <c r="V19" s="274"/>
-      <c r="W19" s="274"/>
+      <c r="Q19" s="314"/>
+      <c r="R19" s="274"/>
+      <c r="S19" s="274"/>
+      <c r="T19" s="274"/>
+      <c r="U19" s="275"/>
+      <c r="V19" s="275"/>
+      <c r="W19" s="275"/>
       <c r="X19" s="273"/>
       <c r="Y19" s="273"/>
       <c r="AN19" s="236"/>
     </row>
     <row r="20" spans="1:40" s="234" customFormat="1" ht="37.5" customHeight="1">
       <c r="B20" s="277" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="C20" s="277"/>
       <c r="D20" s="277" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="E20" s="277"/>
       <c r="F20" s="277"/>
@@ -19614,20 +19625,20 @@
       <c r="I20" s="277"/>
       <c r="J20" s="277"/>
       <c r="K20" s="277"/>
-      <c r="L20" s="284" t="s">
+      <c r="L20" s="281" t="s">
         <v>24</v>
       </c>
-      <c r="M20" s="284"/>
-      <c r="N20" s="284"/>
-      <c r="O20" s="284"/>
-      <c r="P20" s="284"/>
-      <c r="Q20" s="284"/>
-      <c r="R20" s="275"/>
-      <c r="S20" s="275"/>
-      <c r="T20" s="275"/>
-      <c r="U20" s="274"/>
-      <c r="V20" s="274"/>
-      <c r="W20" s="274"/>
+      <c r="M20" s="281"/>
+      <c r="N20" s="281"/>
+      <c r="O20" s="281"/>
+      <c r="P20" s="281"/>
+      <c r="Q20" s="281"/>
+      <c r="R20" s="274"/>
+      <c r="S20" s="274"/>
+      <c r="T20" s="274"/>
+      <c r="U20" s="275"/>
+      <c r="V20" s="275"/>
+      <c r="W20" s="275"/>
       <c r="X20" s="273" t="s">
         <v>60</v>
       </c>
@@ -19635,12 +19646,12 @@
       <c r="AN20" s="237"/>
     </row>
     <row r="21" spans="1:40" s="209" customFormat="1" ht="22.7" customHeight="1">
-      <c r="B21" s="279" t="s">
+      <c r="B21" s="283" t="s">
         <v>26</v>
       </c>
-      <c r="C21" s="280"/>
+      <c r="C21" s="284"/>
       <c r="D21" s="276" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="E21" s="276"/>
       <c r="F21" s="276"/>
@@ -19650,19 +19661,19 @@
       <c r="J21" s="276"/>
       <c r="K21" s="276"/>
       <c r="L21" s="276" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="M21" s="276"/>
       <c r="N21" s="276"/>
       <c r="O21" s="276"/>
       <c r="P21" s="276"/>
       <c r="Q21" s="276"/>
-      <c r="R21" s="275"/>
-      <c r="S21" s="275"/>
-      <c r="T21" s="275"/>
-      <c r="U21" s="274"/>
-      <c r="V21" s="274"/>
-      <c r="W21" s="274"/>
+      <c r="R21" s="274"/>
+      <c r="S21" s="274"/>
+      <c r="T21" s="274"/>
+      <c r="U21" s="275"/>
+      <c r="V21" s="275"/>
+      <c r="W21" s="275"/>
       <c r="X21" s="273" t="s">
         <v>60</v>
       </c>
@@ -19670,10 +19681,10 @@
       <c r="AN21" s="238"/>
     </row>
     <row r="22" spans="1:40" s="209" customFormat="1" ht="22.7" customHeight="1">
-      <c r="B22" s="279" t="s">
+      <c r="B22" s="283" t="s">
         <v>27</v>
       </c>
-      <c r="C22" s="280"/>
+      <c r="C22" s="284"/>
       <c r="D22" s="276"/>
       <c r="E22" s="276"/>
       <c r="F22" s="276"/>
@@ -19688,12 +19699,12 @@
       <c r="O22" s="276"/>
       <c r="P22" s="276"/>
       <c r="Q22" s="276"/>
-      <c r="R22" s="275"/>
-      <c r="S22" s="275"/>
-      <c r="T22" s="275"/>
-      <c r="U22" s="274"/>
-      <c r="V22" s="274"/>
-      <c r="W22" s="274"/>
+      <c r="R22" s="274"/>
+      <c r="S22" s="274"/>
+      <c r="T22" s="274"/>
+      <c r="U22" s="275"/>
+      <c r="V22" s="275"/>
+      <c r="W22" s="275"/>
       <c r="X22" s="273" t="s">
         <v>60</v>
       </c>
@@ -19701,10 +19712,10 @@
       <c r="AN22" s="238"/>
     </row>
     <row r="23" spans="1:40" s="209" customFormat="1" ht="22.7" customHeight="1">
-      <c r="B23" s="279" t="s">
+      <c r="B23" s="283" t="s">
         <v>28</v>
       </c>
-      <c r="C23" s="280"/>
+      <c r="C23" s="284"/>
       <c r="D23" s="276"/>
       <c r="E23" s="276"/>
       <c r="F23" s="276"/>
@@ -19719,12 +19730,12 @@
       <c r="O23" s="276"/>
       <c r="P23" s="276"/>
       <c r="Q23" s="276"/>
-      <c r="R23" s="275"/>
-      <c r="S23" s="275"/>
-      <c r="T23" s="275"/>
-      <c r="U23" s="274"/>
-      <c r="V23" s="274"/>
-      <c r="W23" s="274"/>
+      <c r="R23" s="274"/>
+      <c r="S23" s="274"/>
+      <c r="T23" s="274"/>
+      <c r="U23" s="275"/>
+      <c r="V23" s="275"/>
+      <c r="W23" s="275"/>
       <c r="X23" s="273" t="s">
         <v>60</v>
       </c>
@@ -19732,10 +19743,10 @@
       <c r="AN23" s="238"/>
     </row>
     <row r="24" spans="1:40" s="209" customFormat="1" ht="22.7" customHeight="1">
-      <c r="B24" s="279" t="s">
+      <c r="B24" s="283" t="s">
         <v>29</v>
       </c>
-      <c r="C24" s="280"/>
+      <c r="C24" s="284"/>
       <c r="D24" s="276"/>
       <c r="E24" s="276"/>
       <c r="F24" s="276"/>
@@ -19750,12 +19761,12 @@
       <c r="O24" s="276"/>
       <c r="P24" s="276"/>
       <c r="Q24" s="276"/>
-      <c r="R24" s="275"/>
-      <c r="S24" s="275"/>
-      <c r="T24" s="275"/>
-      <c r="U24" s="274"/>
-      <c r="V24" s="274"/>
-      <c r="W24" s="274"/>
+      <c r="R24" s="274"/>
+      <c r="S24" s="274"/>
+      <c r="T24" s="274"/>
+      <c r="U24" s="275"/>
+      <c r="V24" s="275"/>
+      <c r="W24" s="275"/>
       <c r="X24" s="273" t="s">
         <v>60</v>
       </c>
@@ -19763,10 +19774,10 @@
       <c r="AN24" s="238"/>
     </row>
     <row r="25" spans="1:40" s="209" customFormat="1" ht="22.7" customHeight="1">
-      <c r="B25" s="279" t="s">
+      <c r="B25" s="283" t="s">
         <v>30</v>
       </c>
-      <c r="C25" s="280"/>
+      <c r="C25" s="284"/>
       <c r="D25" s="276"/>
       <c r="E25" s="276"/>
       <c r="F25" s="276"/>
@@ -19781,12 +19792,12 @@
       <c r="O25" s="276"/>
       <c r="P25" s="276"/>
       <c r="Q25" s="276"/>
-      <c r="R25" s="275"/>
-      <c r="S25" s="275"/>
-      <c r="T25" s="275"/>
-      <c r="U25" s="274"/>
-      <c r="V25" s="274"/>
-      <c r="W25" s="274"/>
+      <c r="R25" s="274"/>
+      <c r="S25" s="274"/>
+      <c r="T25" s="274"/>
+      <c r="U25" s="275"/>
+      <c r="V25" s="275"/>
+      <c r="W25" s="275"/>
       <c r="X25" s="273" t="s">
         <v>60</v>
       </c>
@@ -19798,33 +19809,33 @@
         <v>36</v>
       </c>
       <c r="C26" s="277" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="D26" s="277"/>
       <c r="E26" s="277" t="s">
+        <v>283</v>
+      </c>
+      <c r="F26" s="282" t="s">
         <v>284</v>
       </c>
-      <c r="F26" s="278" t="s">
+      <c r="G26" s="282"/>
+      <c r="H26" s="282"/>
+      <c r="I26" s="282"/>
+      <c r="J26" s="282"/>
+      <c r="K26" s="282"/>
+      <c r="L26" s="350" t="s">
         <v>285</v>
-      </c>
-      <c r="G26" s="278"/>
-      <c r="H26" s="278"/>
-      <c r="I26" s="278"/>
-      <c r="J26" s="278"/>
-      <c r="K26" s="278"/>
-      <c r="L26" s="350" t="s">
-        <v>286</v>
       </c>
       <c r="M26" s="351"/>
       <c r="N26" s="349" t="s">
+        <v>286</v>
+      </c>
+      <c r="O26" s="349" t="s">
         <v>287</v>
-      </c>
-      <c r="O26" s="349" t="s">
-        <v>288</v>
       </c>
       <c r="P26" s="349"/>
       <c r="Q26" s="350" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="R26" s="354"/>
       <c r="S26" s="354"/>
@@ -19838,18 +19849,18 @@
     <row r="27" spans="1:40" ht="41.25" customHeight="1">
       <c r="B27" s="277"/>
       <c r="C27" s="240" t="s">
+        <v>281</v>
+      </c>
+      <c r="D27" s="240" t="s">
         <v>282</v>
       </c>
-      <c r="D27" s="240" t="s">
-        <v>283</v>
-      </c>
       <c r="E27" s="277"/>
-      <c r="F27" s="278"/>
-      <c r="G27" s="278"/>
-      <c r="H27" s="278"/>
-      <c r="I27" s="278"/>
-      <c r="J27" s="278"/>
-      <c r="K27" s="278"/>
+      <c r="F27" s="282"/>
+      <c r="G27" s="282"/>
+      <c r="H27" s="282"/>
+      <c r="I27" s="282"/>
+      <c r="J27" s="282"/>
+      <c r="K27" s="282"/>
       <c r="L27" s="352"/>
       <c r="M27" s="353"/>
       <c r="N27" s="349"/>
@@ -19873,13 +19884,13 @@
         <v>26</v>
       </c>
       <c r="D28" s="243" t="s">
+        <v>299</v>
+      </c>
+      <c r="E28" s="244" t="s">
+        <v>295</v>
+      </c>
+      <c r="F28" s="264" t="s">
         <v>300</v>
-      </c>
-      <c r="E28" s="244" t="s">
-        <v>296</v>
-      </c>
-      <c r="F28" s="264" t="s">
-        <v>301</v>
       </c>
       <c r="G28" s="265"/>
       <c r="H28" s="265"/>
@@ -19893,12 +19904,14 @@
         <v>256</v>
       </c>
       <c r="N28" s="239" t="s">
-        <v>302</v>
-      </c>
-      <c r="O28" s="266"/>
+        <v>301</v>
+      </c>
+      <c r="O28" s="266">
+        <v>43036</v>
+      </c>
       <c r="P28" s="267"/>
       <c r="Q28" s="270" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="R28" s="271"/>
       <c r="S28" s="271"/>
@@ -19917,13 +19930,13 @@
         <v>26</v>
       </c>
       <c r="D29" s="243" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="E29" s="244" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="F29" s="264" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="G29" s="265"/>
       <c r="H29" s="265"/>
@@ -19937,12 +19950,14 @@
         <v>256</v>
       </c>
       <c r="N29" s="239" t="s">
-        <v>302</v>
-      </c>
-      <c r="O29" s="266"/>
+        <v>301</v>
+      </c>
+      <c r="O29" s="266">
+        <v>43036</v>
+      </c>
       <c r="P29" s="267"/>
       <c r="Q29" s="270" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="R29" s="271"/>
       <c r="S29" s="271"/>
@@ -19961,13 +19976,13 @@
         <v>26</v>
       </c>
       <c r="D30" s="243" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="E30" s="244" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="F30" s="264" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="G30" s="265"/>
       <c r="H30" s="265"/>
@@ -19978,15 +19993,17 @@
         <v>255</v>
       </c>
       <c r="M30" s="246" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="N30" s="239" t="s">
-        <v>302</v>
-      </c>
-      <c r="O30" s="266"/>
+        <v>301</v>
+      </c>
+      <c r="O30" s="266">
+        <v>43036</v>
+      </c>
       <c r="P30" s="267"/>
       <c r="Q30" s="270" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="R30" s="271"/>
       <c r="S30" s="271"/>
@@ -20005,13 +20022,13 @@
         <v>26</v>
       </c>
       <c r="D31" s="243" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="E31" s="244" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="F31" s="264" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="G31" s="265"/>
       <c r="H31" s="265"/>
@@ -20022,15 +20039,17 @@
         <v>255</v>
       </c>
       <c r="M31" s="246" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="N31" s="239" t="s">
-        <v>302</v>
-      </c>
-      <c r="O31" s="266"/>
+        <v>301</v>
+      </c>
+      <c r="O31" s="266">
+        <v>43036</v>
+      </c>
       <c r="P31" s="267"/>
       <c r="Q31" s="270" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="R31" s="271"/>
       <c r="S31" s="271"/>
@@ -20049,13 +20068,13 @@
         <v>26</v>
       </c>
       <c r="D32" s="243" t="s">
+        <v>312</v>
+      </c>
+      <c r="E32" s="244" t="s">
+        <v>295</v>
+      </c>
+      <c r="F32" s="264" t="s">
         <v>313</v>
-      </c>
-      <c r="E32" s="244" t="s">
-        <v>296</v>
-      </c>
-      <c r="F32" s="264" t="s">
-        <v>314</v>
       </c>
       <c r="G32" s="265"/>
       <c r="H32" s="265"/>
@@ -20069,12 +20088,14 @@
         <v>256</v>
       </c>
       <c r="N32" s="239" t="s">
-        <v>302</v>
-      </c>
-      <c r="O32" s="266"/>
+        <v>301</v>
+      </c>
+      <c r="O32" s="266">
+        <v>43036</v>
+      </c>
       <c r="P32" s="267"/>
       <c r="Q32" s="270" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="R32" s="271"/>
       <c r="S32" s="271"/>
@@ -20093,13 +20114,13 @@
         <v>26</v>
       </c>
       <c r="D33" s="243" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="E33" s="244" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="F33" s="264" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="G33" s="265"/>
       <c r="H33" s="265"/>
@@ -20113,12 +20134,14 @@
         <v>256</v>
       </c>
       <c r="N33" s="239" t="s">
-        <v>302</v>
-      </c>
-      <c r="O33" s="266"/>
+        <v>301</v>
+      </c>
+      <c r="O33" s="266">
+        <v>43036</v>
+      </c>
       <c r="P33" s="267"/>
       <c r="Q33" s="270" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="R33" s="271"/>
       <c r="S33" s="271"/>
@@ -20137,13 +20160,13 @@
         <v>26</v>
       </c>
       <c r="D34" s="243" t="s">
+        <v>322</v>
+      </c>
+      <c r="E34" s="244" t="s">
         <v>323</v>
       </c>
-      <c r="E34" s="244" t="s">
-        <v>324</v>
-      </c>
       <c r="F34" s="264" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="G34" s="265"/>
       <c r="H34" s="265"/>
@@ -20154,15 +20177,17 @@
         <v>255</v>
       </c>
       <c r="M34" s="246" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="N34" s="239" t="s">
-        <v>326</v>
-      </c>
-      <c r="O34" s="266"/>
+        <v>325</v>
+      </c>
+      <c r="O34" s="266">
+        <v>43036</v>
+      </c>
       <c r="P34" s="267"/>
       <c r="Q34" s="270" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="R34" s="271"/>
       <c r="S34" s="271"/>
@@ -20175,19 +20200,19 @@
     </row>
     <row r="35" spans="1:26" ht="52.5" customHeight="1">
       <c r="B35" s="241">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="C35" s="242" t="s">
         <v>26</v>
       </c>
       <c r="D35" s="243" t="s">
+        <v>327</v>
+      </c>
+      <c r="E35" s="244" t="s">
+        <v>323</v>
+      </c>
+      <c r="F35" s="264" t="s">
         <v>328</v>
-      </c>
-      <c r="E35" s="244" t="s">
-        <v>324</v>
-      </c>
-      <c r="F35" s="264" t="s">
-        <v>329</v>
       </c>
       <c r="G35" s="265"/>
       <c r="H35" s="265"/>
@@ -20201,12 +20226,14 @@
         <v>256</v>
       </c>
       <c r="N35" s="239" t="s">
-        <v>326</v>
-      </c>
-      <c r="O35" s="266"/>
+        <v>325</v>
+      </c>
+      <c r="O35" s="266">
+        <v>43036</v>
+      </c>
       <c r="P35" s="267"/>
       <c r="Q35" s="270" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="R35" s="271"/>
       <c r="S35" s="271"/>
@@ -20220,19 +20247,19 @@
     <row r="36" spans="1:26" ht="42" customHeight="1">
       <c r="A36" s="233"/>
       <c r="B36" s="241">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="C36" s="242" t="s">
         <v>26</v>
       </c>
       <c r="D36" s="243" t="s">
+        <v>330</v>
+      </c>
+      <c r="E36" s="244" t="s">
+        <v>323</v>
+      </c>
+      <c r="F36" s="264" t="s">
         <v>331</v>
-      </c>
-      <c r="E36" s="244" t="s">
-        <v>324</v>
-      </c>
-      <c r="F36" s="264" t="s">
-        <v>332</v>
       </c>
       <c r="G36" s="265"/>
       <c r="H36" s="265"/>
@@ -20246,12 +20273,14 @@
         <v>256</v>
       </c>
       <c r="N36" s="239" t="s">
-        <v>326</v>
-      </c>
-      <c r="O36" s="266"/>
+        <v>325</v>
+      </c>
+      <c r="O36" s="266">
+        <v>43036</v>
+      </c>
       <c r="P36" s="267"/>
       <c r="Q36" s="270" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="R36" s="271"/>
       <c r="S36" s="271"/>
@@ -20266,19 +20295,19 @@
     <row r="37" spans="1:26" ht="42" customHeight="1">
       <c r="A37" s="233"/>
       <c r="B37" s="241">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="C37" s="242" t="s">
         <v>26</v>
       </c>
       <c r="D37" s="243" t="s">
+        <v>339</v>
+      </c>
+      <c r="E37" s="244" t="s">
+        <v>323</v>
+      </c>
+      <c r="F37" s="264" t="s">
         <v>340</v>
-      </c>
-      <c r="E37" s="244" t="s">
-        <v>324</v>
-      </c>
-      <c r="F37" s="264" t="s">
-        <v>341</v>
       </c>
       <c r="G37" s="265"/>
       <c r="H37" s="265"/>
@@ -20292,12 +20321,14 @@
         <v>256</v>
       </c>
       <c r="N37" s="239" t="s">
-        <v>326</v>
-      </c>
-      <c r="O37" s="266"/>
+        <v>325</v>
+      </c>
+      <c r="O37" s="266">
+        <v>43036</v>
+      </c>
       <c r="P37" s="267"/>
       <c r="Q37" s="270" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="R37" s="271"/>
       <c r="S37" s="271"/>
@@ -20312,19 +20343,19 @@
     <row r="38" spans="1:26" ht="42" customHeight="1">
       <c r="A38" s="233"/>
       <c r="B38" s="241">
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="C38" s="242" t="s">
         <v>26</v>
       </c>
       <c r="D38" s="243" t="s">
+        <v>332</v>
+      </c>
+      <c r="E38" s="244" t="s">
         <v>333</v>
       </c>
-      <c r="E38" s="244" t="s">
+      <c r="F38" s="264" t="s">
         <v>334</v>
-      </c>
-      <c r="F38" s="264" t="s">
-        <v>335</v>
       </c>
       <c r="G38" s="265"/>
       <c r="H38" s="265"/>
@@ -20338,12 +20369,14 @@
         <v>256</v>
       </c>
       <c r="N38" s="239" t="s">
-        <v>302</v>
-      </c>
-      <c r="O38" s="266"/>
+        <v>301</v>
+      </c>
+      <c r="O38" s="266">
+        <v>43036</v>
+      </c>
       <c r="P38" s="267"/>
       <c r="Q38" s="270" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="R38" s="271"/>
       <c r="S38" s="271"/>
@@ -20358,19 +20391,19 @@
     <row r="39" spans="1:26" s="251" customFormat="1" ht="42" customHeight="1">
       <c r="A39" s="250"/>
       <c r="B39" s="241">
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="C39" s="242" t="s">
         <v>26</v>
       </c>
       <c r="D39" s="243" t="s">
+        <v>336</v>
+      </c>
+      <c r="E39" s="244" t="s">
+        <v>333</v>
+      </c>
+      <c r="F39" s="264" t="s">
         <v>337</v>
-      </c>
-      <c r="E39" s="244" t="s">
-        <v>334</v>
-      </c>
-      <c r="F39" s="264" t="s">
-        <v>338</v>
       </c>
       <c r="G39" s="265"/>
       <c r="H39" s="265"/>
@@ -20384,12 +20417,14 @@
         <v>256</v>
       </c>
       <c r="N39" s="239" t="s">
-        <v>302</v>
-      </c>
-      <c r="O39" s="266"/>
+        <v>301</v>
+      </c>
+      <c r="O39" s="266">
+        <v>43036</v>
+      </c>
       <c r="P39" s="267"/>
       <c r="Q39" s="270" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="R39" s="271"/>
       <c r="S39" s="271"/>
@@ -21685,6 +21720,19 @@
   </sheetData>
   <dataConsolidate/>
   <mergeCells count="258">
+    <mergeCell ref="X19:Y19"/>
+    <mergeCell ref="U22:W22"/>
+    <mergeCell ref="X20:Y20"/>
+    <mergeCell ref="R22:T22"/>
+    <mergeCell ref="U24:W24"/>
+    <mergeCell ref="X17:Y17"/>
+    <mergeCell ref="H17:Q17"/>
+    <mergeCell ref="H18:I18"/>
+    <mergeCell ref="P18:Q18"/>
+    <mergeCell ref="U16:Y16"/>
+    <mergeCell ref="F18:G18"/>
+    <mergeCell ref="U18:W18"/>
+    <mergeCell ref="X18:Y18"/>
     <mergeCell ref="Q39:V39"/>
     <mergeCell ref="R19:T19"/>
     <mergeCell ref="Q34:V34"/>
@@ -21700,7 +21748,7 @@
     <mergeCell ref="Q28:V28"/>
     <mergeCell ref="Q30:V30"/>
     <mergeCell ref="X26:Y26"/>
-    <mergeCell ref="R18:T18"/>
+    <mergeCell ref="U23:W23"/>
     <mergeCell ref="Q1:S1"/>
     <mergeCell ref="T1:Y1"/>
     <mergeCell ref="G3:I3"/>
@@ -21716,17 +21764,6 @@
     <mergeCell ref="W8:Y12"/>
     <mergeCell ref="T3:Y3"/>
     <mergeCell ref="T8:V12"/>
-    <mergeCell ref="X17:Y17"/>
-    <mergeCell ref="H17:Q17"/>
-    <mergeCell ref="H18:I18"/>
-    <mergeCell ref="P18:Q18"/>
-    <mergeCell ref="U23:W23"/>
-    <mergeCell ref="U16:Y16"/>
-    <mergeCell ref="F18:G18"/>
-    <mergeCell ref="U18:W18"/>
-    <mergeCell ref="B19:E19"/>
-    <mergeCell ref="F19:G19"/>
-    <mergeCell ref="H19:I19"/>
     <mergeCell ref="R17:T17"/>
     <mergeCell ref="U19:W19"/>
     <mergeCell ref="B16:E17"/>
@@ -21742,8 +21779,9 @@
     <mergeCell ref="P19:Q19"/>
     <mergeCell ref="F17:G17"/>
     <mergeCell ref="J19:K19"/>
-    <mergeCell ref="X18:Y18"/>
-    <mergeCell ref="D20:K20"/>
+    <mergeCell ref="R16:T16"/>
+    <mergeCell ref="U17:W17"/>
+    <mergeCell ref="R18:T18"/>
     <mergeCell ref="T7:V7"/>
     <mergeCell ref="J3:O3"/>
     <mergeCell ref="G10:I10"/>
@@ -21753,8 +21791,6 @@
     <mergeCell ref="J5:O6"/>
     <mergeCell ref="J8:O8"/>
     <mergeCell ref="J10:O10"/>
-    <mergeCell ref="R16:T16"/>
-    <mergeCell ref="X40:Y40"/>
     <mergeCell ref="X21:Y21"/>
     <mergeCell ref="B25:C25"/>
     <mergeCell ref="D25:K25"/>
@@ -21773,14 +21809,10 @@
     <mergeCell ref="B24:C24"/>
     <mergeCell ref="R23:T23"/>
     <mergeCell ref="B20:C20"/>
-    <mergeCell ref="U17:W17"/>
     <mergeCell ref="B21:C21"/>
     <mergeCell ref="D22:K22"/>
     <mergeCell ref="R21:T21"/>
-    <mergeCell ref="F36:K36"/>
-    <mergeCell ref="O36:P36"/>
-    <mergeCell ref="O35:P35"/>
-    <mergeCell ref="O37:P37"/>
+    <mergeCell ref="D20:K20"/>
     <mergeCell ref="B26:B27"/>
     <mergeCell ref="P16:Q16"/>
     <mergeCell ref="H16:I16"/>
@@ -21797,11 +21829,9 @@
     <mergeCell ref="F26:K27"/>
     <mergeCell ref="B23:C23"/>
     <mergeCell ref="D23:K23"/>
-    <mergeCell ref="X19:Y19"/>
-    <mergeCell ref="U22:W22"/>
-    <mergeCell ref="X20:Y20"/>
-    <mergeCell ref="R22:T22"/>
-    <mergeCell ref="U24:W24"/>
+    <mergeCell ref="B19:E19"/>
+    <mergeCell ref="F19:G19"/>
+    <mergeCell ref="H19:I19"/>
     <mergeCell ref="X24:Y24"/>
     <mergeCell ref="F39:K39"/>
     <mergeCell ref="O39:P39"/>
@@ -21824,6 +21854,16 @@
     <mergeCell ref="X38:Y38"/>
     <mergeCell ref="F37:K37"/>
     <mergeCell ref="X28:Y28"/>
+    <mergeCell ref="Q37:V37"/>
+    <mergeCell ref="Q38:V38"/>
+    <mergeCell ref="F31:K31"/>
+    <mergeCell ref="Q29:V29"/>
+    <mergeCell ref="Q31:V31"/>
+    <mergeCell ref="F43:K43"/>
+    <mergeCell ref="O43:P43"/>
+    <mergeCell ref="X42:Y42"/>
+    <mergeCell ref="O54:P54"/>
+    <mergeCell ref="X49:Y49"/>
     <mergeCell ref="F51:K51"/>
     <mergeCell ref="O51:P51"/>
     <mergeCell ref="X46:Y46"/>
@@ -21835,21 +21875,20 @@
     <mergeCell ref="O45:P45"/>
     <mergeCell ref="F46:K46"/>
     <mergeCell ref="O46:P46"/>
-    <mergeCell ref="Q37:V37"/>
-    <mergeCell ref="Q38:V38"/>
+    <mergeCell ref="X40:Y40"/>
+    <mergeCell ref="F36:K36"/>
+    <mergeCell ref="O36:P36"/>
+    <mergeCell ref="O35:P35"/>
+    <mergeCell ref="O37:P37"/>
+    <mergeCell ref="X44:Y44"/>
+    <mergeCell ref="F52:K52"/>
+    <mergeCell ref="O52:P52"/>
+    <mergeCell ref="F49:K49"/>
+    <mergeCell ref="F50:K50"/>
+    <mergeCell ref="O50:P50"/>
+    <mergeCell ref="X45:Y45"/>
+    <mergeCell ref="X53:Y53"/>
     <mergeCell ref="X37:Y37"/>
-    <mergeCell ref="X36:Y36"/>
-    <mergeCell ref="F31:K31"/>
-    <mergeCell ref="Q29:V29"/>
-    <mergeCell ref="Q31:V31"/>
-    <mergeCell ref="F43:K43"/>
-    <mergeCell ref="O43:P43"/>
-    <mergeCell ref="X42:Y42"/>
-    <mergeCell ref="O54:P54"/>
-    <mergeCell ref="X49:Y49"/>
-    <mergeCell ref="F55:K55"/>
-    <mergeCell ref="X56:Y56"/>
-    <mergeCell ref="F42:K42"/>
     <mergeCell ref="Q32:V32"/>
     <mergeCell ref="O42:P42"/>
     <mergeCell ref="F40:K40"/>
@@ -21862,16 +21901,7 @@
     <mergeCell ref="X34:Y34"/>
     <mergeCell ref="O40:P40"/>
     <mergeCell ref="Q33:V33"/>
-    <mergeCell ref="X44:Y44"/>
-    <mergeCell ref="F52:K52"/>
-    <mergeCell ref="O52:P52"/>
-    <mergeCell ref="F49:K49"/>
-    <mergeCell ref="F50:K50"/>
-    <mergeCell ref="O50:P50"/>
-    <mergeCell ref="X45:Y45"/>
-    <mergeCell ref="X53:Y53"/>
-    <mergeCell ref="F59:K59"/>
-    <mergeCell ref="O59:P59"/>
+    <mergeCell ref="X36:Y36"/>
     <mergeCell ref="X54:Y54"/>
     <mergeCell ref="O57:P57"/>
     <mergeCell ref="F57:K57"/>
@@ -21893,6 +21923,9 @@
     <mergeCell ref="X51:Y51"/>
     <mergeCell ref="X55:Y55"/>
     <mergeCell ref="F54:K54"/>
+    <mergeCell ref="F55:K55"/>
+    <mergeCell ref="X56:Y56"/>
+    <mergeCell ref="F42:K42"/>
     <mergeCell ref="X60:Y60"/>
     <mergeCell ref="F62:K62"/>
     <mergeCell ref="O62:P62"/>
@@ -21906,6 +21939,8 @@
     <mergeCell ref="O61:P61"/>
     <mergeCell ref="F58:K58"/>
     <mergeCell ref="O58:P58"/>
+    <mergeCell ref="F59:K59"/>
+    <mergeCell ref="O59:P59"/>
     <mergeCell ref="F68:K68"/>
     <mergeCell ref="O68:P68"/>
     <mergeCell ref="X63:Y63"/>
@@ -21969,7 +22004,7 @@
   </dataValidations>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.39370078740157483" right="0.39370078740157483" top="0.59055118110236227" bottom="0.39370078740157483" header="0.31496062992125984" footer="0.19685039370078741"/>
-  <pageSetup paperSize="9" scale="61" fitToHeight="0" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" scale="62" fitToHeight="0" orientation="portrait" r:id="rId1"/>
   <headerFooter scaleWithDoc="0" alignWithMargins="0">
     <oddFooter>&amp;C&amp;9&amp;P/&amp;N</oddFooter>
   </headerFooter>
@@ -26686,7 +26721,7 @@
   </dataValidations>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.39370078740157483" right="0.39370078740157483" top="0.59055118110236227" bottom="0.39370078740157483" header="0.31496062992125984" footer="0.19685039370078741"/>
-  <pageSetup paperSize="9" scale="68" fitToHeight="0" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" scale="67" fitToHeight="0" orientation="portrait" r:id="rId1"/>
   <headerFooter alignWithMargins="0">
     <oddFooter>&amp;C&amp;9&amp;P/&amp;N</oddFooter>
   </headerFooter>

</xml_diff>